<commit_message>
add package Utils + read Data for FB
</commit_message>
<xml_diff>
--- a/TestAuto/DataTest/DataAutoFB.xlsx
+++ b/TestAuto/DataTest/DataAutoFB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NTLNEO\git\CoreAutomationTest\TestAuto\DataTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\CoreAutomationTest\TestAuto\DataTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9983E79-C3F7-47A5-8B06-307EFE3C1DAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D2B57F-B5FD-4E00-BBBD-36E9A63D3E10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26985" yWindow="2040" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Like4Like" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
   <si>
     <t>#</t>
   </si>
@@ -400,16 +400,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" customWidth="1"/>
   </cols>
@@ -436,9 +436,17 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -454,7 +462,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add more acc to Excel
</commit_message>
<xml_diff>
--- a/TestAuto/DataTest/DataAutoFB.xlsx
+++ b/TestAuto/DataTest/DataAutoFB.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NTLNEO\git\CoreAutomationTest\TestAuto\DataTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\CoreAutomationTest\TestAuto\DataTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83963B46-39DC-41B3-899A-88A3DCB122C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535CD753-17B2-4082-B0C5-530F547B9799}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26985" yWindow="2040" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Like4Like" sheetId="1" r:id="rId1"/>
     <sheet name="FB" sheetId="2" r:id="rId2"/>
     <sheet name="Google" sheetId="3" r:id="rId3"/>
+    <sheet name="FB rieng" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
   <si>
     <t>#</t>
   </si>
@@ -47,47 +48,97 @@
     <t>Password</t>
   </si>
   <si>
+    <t>an.thanh282000@gmail.com</t>
+  </si>
+  <si>
+    <t>Docnhat001@</t>
+  </si>
+  <si>
+    <t>lamnguyeneditor@gmail.com</t>
+  </si>
+  <si>
+    <t>lamnguyeneditor1@gmail.com</t>
+  </si>
+  <si>
+    <t>Xzsawq8487!@#</t>
+  </si>
+  <si>
+    <t>suzukihzt@gmail.com</t>
+  </si>
+  <si>
+    <t>Docnhat1</t>
+  </si>
+  <si>
+    <t>phungtest04@gmail.com</t>
+  </si>
+  <si>
+    <t>phung123</t>
+  </si>
+  <si>
+    <t>suzukihzt</t>
+  </si>
+  <si>
+    <t>judytrinh2609@gmail.com</t>
+  </si>
+  <si>
+    <t>35nguyenhue</t>
+  </si>
+  <si>
+    <t>tamhuynhnh@gmail.com</t>
+  </si>
+  <si>
+    <t>maichitrinhtran@gmail.com</t>
+  </si>
+  <si>
+    <t>thithipleple@gmail.com</t>
+  </si>
+  <si>
+    <t>hngtrnthnhhng@gmail.com</t>
+  </si>
+  <si>
+    <t>anthuynhien267@gmail.com</t>
+  </si>
+  <si>
+    <t>35Nguyenhue</t>
+  </si>
+  <si>
     <t>ntlneo</t>
   </si>
   <si>
-    <t>an.thanh282000@gmail.com</t>
-  </si>
-  <si>
-    <t>Docnhat001@</t>
-  </si>
-  <si>
-    <t>lamnguyeneditor@gmail.com</t>
-  </si>
-  <si>
-    <t>lamnguyeneditor1@gmail.com</t>
-  </si>
-  <si>
-    <t>Xzsawq8487!@#</t>
-  </si>
-  <si>
-    <t>suzukihzt@gmail.com</t>
-  </si>
-  <si>
-    <t>Docnhat1</t>
-  </si>
-  <si>
-    <t>phungtest04@gmail.com</t>
-  </si>
-  <si>
-    <t>phung123</t>
-  </si>
-  <si>
-    <t>suzukihzt</t>
+    <t>353535</t>
+  </si>
+  <si>
+    <t>echconcutecute@gmail.com</t>
+  </si>
+  <si>
+    <t>tudangnhap12345</t>
+  </si>
+  <si>
+    <t>fancythiezhang@gmail.com</t>
+  </si>
+  <si>
+    <t>caphemot2345@gmail.com</t>
+  </si>
+  <si>
+    <t>caphe12345</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -107,7 +158,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -115,16 +166,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -405,9 +480,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,33 +514,36 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{9BC9F410-A902-461E-A752-99DDB9809472}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD819D16-1434-4D66-B4ED-8A727D9A3231}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +554,7 @@
     <col min="5" max="5" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,36 +574,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -573,34 +643,34 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -611,4 +681,128 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC6EF19-363F-4755-86A3-0F2A3FA394D5}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
upadte acc and numb
</commit_message>
<xml_diff>
--- a/TestAuto/DataTest/DataAutoFB.xlsx
+++ b/TestAuto/DataTest/DataAutoFB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\CoreAutomationTest\TestAuto\DataTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535CD753-17B2-4082-B0C5-530F547B9799}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C062AB6D-F71C-4456-B708-76F79C634F57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -539,11 +539,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD819D16-1434-4D66-B4ED-8A727D9A3231}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,26 +576,50 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>30</v>
+        <v>19</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -689,7 +713,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12:C13"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,51 +779,39 @@
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
clear sleep and fix bug login and like post
</commit_message>
<xml_diff>
--- a/TestAuto/DataTest/DataAutoFB.xlsx
+++ b/TestAuto/DataTest/DataAutoFB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\CoreAutomationTest\TestAuto\DataTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NTLNEO\git\CoreAutomationTest\TestAuto\DataTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFB3054-0340-40DA-B774-DB31AF320D30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2170BA-381C-4F6A-AA5F-16455DB422E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26985" yWindow="2040" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Like4Like" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
   <si>
     <t>#</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>353535</t>
-  </si>
-  <si>
-    <t>echconcutecute@gmail.com</t>
   </si>
   <si>
     <t>tudangnhap12345</t>
@@ -536,11 +533,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD819D16-1434-4D66-B4ED-8A727D9A3231}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,74 +570,18 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -655,7 +596,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,11 +671,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC6EF19-363F-4755-86A3-0F2A3FA394D5}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,16 +740,52 @@
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add acc and fix bug
</commit_message>
<xml_diff>
--- a/TestAuto/DataTest/DataAutoFB.xlsx
+++ b/TestAuto/DataTest/DataAutoFB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NTLNEO\git\CoreAutomationTest\TestAuto\DataTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\CoreAutomationTest\TestAuto\DataTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855CD73C-9911-43F7-A4EB-CDF4FF89CDA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D0F0B5-9686-45B3-8005-4EA4EB3772C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26985" yWindow="2040" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2550" windowWidth="20490" windowHeight="8370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Like4Like" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="30">
   <si>
     <t>#</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>FB Lam</t>
+  </si>
+  <si>
+    <t>lameditor1</t>
   </si>
 </sst>
 </file>
@@ -458,11 +461,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +501,7 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
@@ -512,6 +515,17 @@
         <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -525,9 +539,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD819D16-1434-4D66-B4ED-8A727D9A3231}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:C4"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,11 +604,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC6EF19-363F-4755-86A3-0F2A3FA394D5}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,9 +641,41 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -645,7 +691,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14:XFD14"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fix web reload when run doLoopLike
</commit_message>
<xml_diff>
--- a/TestAuto/DataTest/DataAutoFB.xlsx
+++ b/TestAuto/DataTest/DataAutoFB.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NTLNEO\git\CoreAutomationTest\TestAuto\DataTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EB8D40-1B85-42A3-BD1D-7349865C53BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FBD899-27C9-4150-BB5B-643CB225B581}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26985" yWindow="2040" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26985" yWindow="2040" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Like4Like" sheetId="1" r:id="rId1"/>
     <sheet name="FB Lam" sheetId="2" r:id="rId2"/>
     <sheet name="FB Cty" sheetId="4" r:id="rId3"/>
-    <sheet name="Google" sheetId="3" r:id="rId4"/>
+    <sheet name="FB tong" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="29">
   <si>
     <t>#</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>an.thanh282000@gmail.com</t>
-  </si>
-  <si>
     <t>Docnhat001@</t>
   </si>
   <si>
@@ -60,13 +57,7 @@
     <t>lamnguyeneditor1@gmail.com</t>
   </si>
   <si>
-    <t>Xzsawq8487!@#</t>
-  </si>
-  <si>
     <t>suzukihzt@gmail.com</t>
-  </si>
-  <si>
-    <t>Docnhat1</t>
   </si>
   <si>
     <t>phungtest04@gmail.com</t>
@@ -478,9 +469,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +484,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -513,58 +504,59 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -574,11 +566,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD819D16-1434-4D66-B4ED-8A727D9A3231}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,41 +602,59 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -659,7 +669,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,10 +705,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -706,40 +716,34 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>1</v>
-      </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -750,11 +754,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{176F69EE-9456-4E8D-BA54-5D00AF698553}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8:F11"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,7 +770,7 @@
     <col min="6" max="6" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,125 +790,153 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
         <v>8</v>
       </c>
-      <c r="F9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
         <v>9</v>
       </c>
-      <c r="F10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E17" s="3" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{F9B0293E-952C-4BFC-AC69-F283C5FE9D26}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{128D6B85-169A-4243-94BF-707EBBE573D5}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
correct invalid acc FB
</commit_message>
<xml_diff>
--- a/TestAuto/DataTest/DataAutoFB.xlsx
+++ b/TestAuto/DataTest/DataAutoFB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NTLNEO\git\CoreAutomationTest\TestAuto\DataTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\CoreAutomationTest\TestAuto\DataTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8A2245-57EF-4F72-B403-2985A008F715}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D172F4EF-2BE1-421C-8BFE-32F9B9537C58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26985" yWindow="2040" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Like4Like" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="27">
   <si>
     <t>#</t>
   </si>
@@ -463,7 +463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
@@ -501,7 +501,7 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -512,7 +512,7 @@
         <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -560,11 +560,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD819D16-1434-4D66-B4ED-8A727D9A3231}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A2:XFD3"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,7 +575,7 @@
     <col min="5" max="5" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,27 +595,67 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -707,9 +747,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{176F69EE-9456-4E8D-BA54-5D00AF698553}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,70 +845,57 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" t="s">
-        <v>11</v>
-      </c>
-    </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+        <v>25</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>13</v>
+      <c r="E16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
     </row>
     <row r="19" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Android Demo FB work But Selenium Autolike error --> DONT USE selenium-java and appium java-client TO AVOID BUG NoClassDefFound
</commit_message>
<xml_diff>
--- a/TestAuto/DataTest/DataAutoFB.xlsx
+++ b/TestAuto/DataTest/DataAutoFB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\CoreAutomationTest\TestAuto\DataTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NTLNEO\git\CoreAutomationTest\TestAuto\DataTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D172F4EF-2BE1-421C-8BFE-32F9B9537C58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC23DEC-C314-49EF-ABFF-F1D64DB60920}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23205" yWindow="2760" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Like4Like" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="25">
   <si>
     <t>#</t>
   </si>
@@ -58,12 +58,6 @@
   </si>
   <si>
     <t>suzukihzt@gmail.com</t>
-  </si>
-  <si>
-    <t>phungtest04@gmail.com</t>
-  </si>
-  <si>
-    <t>phung123</t>
   </si>
   <si>
     <t>suzukihzt</t>
@@ -463,7 +457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
@@ -478,7 +472,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -498,10 +492,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -509,10 +503,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -520,10 +514,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -531,10 +525,10 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -542,10 +536,10 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>6</v>
@@ -560,11 +554,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD819D16-1434-4D66-B4ED-8A727D9A3231}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:C9"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,7 +569,7 @@
     <col min="5" max="5" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,68 +589,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -707,34 +661,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -745,11 +699,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{176F69EE-9456-4E8D-BA54-5D00AF698553}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12:F16"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,71 +737,71 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="3" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>20</v>
+      <c r="F11" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>6</v>
@@ -855,35 +809,31 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E15" t="s">
+      <c r="E15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E17" s="3"/>
@@ -892,10 +842,6 @@
     <row r="18" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update excel and console
</commit_message>
<xml_diff>
--- a/TestAuto/DataTest/DataAutoFB.xlsx
+++ b/TestAuto/DataTest/DataAutoFB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\CoreAutomationTest\TestAuto\DataTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D172F4EF-2BE1-421C-8BFE-32F9B9537C58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1740BD13-0460-4317-B8D2-2265467B87B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Like4Like" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="25">
   <si>
     <t>#</t>
   </si>
@@ -58,12 +58,6 @@
   </si>
   <si>
     <t>suzukihzt@gmail.com</t>
-  </si>
-  <si>
-    <t>phungtest04@gmail.com</t>
-  </si>
-  <si>
-    <t>phung123</t>
   </si>
   <si>
     <t>suzukihzt</t>
@@ -463,7 +457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
@@ -478,7 +472,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -496,23 +490,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -520,10 +514,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -531,10 +525,10 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
@@ -542,10 +536,10 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>6</v>
@@ -560,11 +554,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD819D16-1434-4D66-B4ED-8A727D9A3231}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:C9"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,42 +591,42 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -640,23 +634,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -671,7 +649,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,34 +685,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -745,11 +723,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{176F69EE-9456-4E8D-BA54-5D00AF698553}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12:F16"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,71 +761,71 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="3" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>20</v>
+      <c r="F11" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>6</v>
@@ -855,35 +833,31 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E15" t="s">
+      <c r="E15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E17" s="3"/>
@@ -892,10 +866,6 @@
     <row r="18" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>